<commit_message>
Corrected order of operations by adding brackets to blackjack
</commit_message>
<xml_diff>
--- a/trainer/softwareJobs.xlsx
+++ b/trainer/softwareJobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>Job Title</t>
   </si>
@@ -25,12 +25,12 @@
     <t>Location</t>
   </si>
   <si>
-    <t xml:space="preserve">Salesforce Systems Developer_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Allen Recruitment Consulting
+    <t xml:space="preserve">Software Developer Technician_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+QA LIMITED
 </t>
   </si>
   <si>
@@ -49,6 +49,24 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Applications Engineer_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Elevation Recruitment
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salesforce Systems Developer_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Allen Recruitment Consulting
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contract Java Developer x 4_x000D_
 </t>
   </si>
@@ -73,7 +91,7 @@
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Salesforce Developer - £55,000 - Leeds_x000D_
+    <t xml:space="preserve">.NET Developer - £62,000 + Bonus - Leeds_x000D_
 </t>
   </si>
   <si>
@@ -91,7 +109,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Java Developer - Leeds_x000D_
+    <t xml:space="preserve">.NET Developer - Global TV Network - Leeds_x000D_
 </t>
   </si>
   <si>
@@ -100,7 +118,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">JavaScript Engineer_x000D_
+    <t xml:space="preserve">Software Engineer_x000D_
 </t>
   </si>
   <si>
@@ -109,39 +127,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Entry-level Information Technology Consultant (Software)_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-QA Consulting
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Front End Focussed Full Stack Developer_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-National Health Service
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-_x000D_
-remote / Leeds, Yorkshire_x000D_
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senior .NET Developer_x000D_
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proclaim Developer - Wakefield, Leeds (West Yorkshire_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">User Acceptance Tester_x000D_
+    <t xml:space="preserve">Software Tester_x000D_
 </t>
   </si>
   <si>
@@ -151,6 +141,10 @@
  </t>
   </si>
   <si>
+    <t xml:space="preserve">Salesforce Developer - £55,000 - Leeds_x000D_
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Senior Software Developer - Salesforce_x000D_
 </t>
   </si>
@@ -159,10 +153,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Software Engineer_x000D_
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remote Ruby on Rails Developer_x000D_
 </t>
   </si>
@@ -171,23 +161,19 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Java Developer - Leeds_x000D_
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Junior .NET Developer_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Software Developer - Video Games C++ C#_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Tester_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote .Net Developer_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DevOps Engineer Security AWS_x000D_
+    <t xml:space="preserve">Software Developer - Salesforce Lightning Java API_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Developer / Engineer Spring RESTful_x000D_
 </t>
   </si>
 </sst>
@@ -529,11 +515,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -587,15 +578,15 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -603,13 +594,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -653,12 +644,12 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -669,32 +660,32 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -702,10 +693,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -713,10 +704,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -724,10 +715,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -735,10 +726,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -746,10 +737,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -757,10 +748,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -768,21 +759,21 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -790,18 +781,18 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -812,10 +803,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -823,23 +814,12 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>